<commit_message>
Added capabilities to load positions and positions assignments from excel file.
</commit_message>
<xml_diff>
--- a/test_data/ldap_data_marvel.xlsx
+++ b/test_data/ldap_data_marvel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t>TINO-NS</t>
   </si>
@@ -216,6 +216,21 @@
   </si>
   <si>
     <t>COMPANY_ID</t>
+  </si>
+  <si>
+    <t>askywalker</t>
+  </si>
+  <si>
+    <t>Anakin</t>
+  </si>
+  <si>
+    <t>Skywalker</t>
+  </si>
+  <si>
+    <t>vader@sith.com</t>
+  </si>
+  <si>
+    <t>200-1234</t>
   </si>
 </sst>
 </file>
@@ -562,7 +577,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="E12" sqref="E12:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -866,6 +881,29 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13">
+        <v>2233355</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -895,6 +933,7 @@
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
     <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>